<commit_message>
add yaml file for Git Action
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataECOM/CustomerDataExcel.xlsx
+++ b/src/test/resources/testdataECOM/CustomerDataExcel.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>VAT</t>
   </si>
@@ -278,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -314,6 +314,48 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -691,7 +733,7 @@
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="32" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="11"/>

</xml_diff>